<commit_message>
Improved results and benchmark testing
</commit_message>
<xml_diff>
--- a/productionalized/articles.xlsx
+++ b/productionalized/articles.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28415"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11207"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sprice/Documents/GitHub/coldSprayTextExtraction/Attempt2/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sprice/Documents/GitHub/coldSprayTextExtraction/productionalized/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="315" documentId="8_{8F8C5BF5-134D-AA45-BDEA-76123C9EFC26}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6B08E811-FA87-4D20-A2B0-5F79FBC0C6A2}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B76A8EE1-476D-A940-9714-BD4C53DC9A52}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1100" yWindow="820" windowWidth="28040" windowHeight="17060" xr2:uid="{175CC6A7-1461-A14D-A5AE-D10584F48326}"/>
+    <workbookView xWindow="1920" yWindow="1100" windowWidth="28040" windowHeight="17060" xr2:uid="{175CC6A7-1461-A14D-A5AE-D10584F48326}"/>
   </bookViews>
   <sheets>
     <sheet name="articles" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="495" uniqueCount="474">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="491" uniqueCount="471">
   <si>
     <t>Index</t>
   </si>
@@ -100,15 +100,6 @@
   </si>
   <si>
     <t>https://www.sciencedirect.com/science/article/pii/S0142112324000100?casa_token=8BTO0UmGmO4AAAAA:mj-VECrBp7wwXChuFvC8pE1aM0gwtxZXrvXa8j56GwyanemaThTVF6jtUgEd1h33433Bo2_c</t>
-  </si>
-  <si>
-    <t>Cold spray process depiction with gas-atomized Al 6061 feedstock ...</t>
-  </si>
-  <si>
-    <t>https://www.researchgate.net/figure/Cold-spray-process-depiction-with-gas-atomized-Al-6061-feedstock-a-is-a-schematic_fig1_344155675</t>
-  </si>
-  <si>
-    <t>... to the point, the orthogonal orientation relative to the cold spray direction of supersonic particle deposition was found to have a lower hardness than the¬†...</t>
   </si>
   <si>
     <t>Ultrasonic and conventional fatigue behavior, strain rate sensitivity, and structural design methods for wrought and cold spray Al-6061</t>
@@ -1510,7 +1501,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="24">
+  <fonts count="24" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -1670,7 +1661,6 @@
       <sz val="12"/>
       <color rgb="FF000000"/>
       <name val="Aptos Narrow"/>
-      <charset val="1"/>
     </font>
     <font>
       <i/>
@@ -2436,17 +2426,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D37F8E98-04D2-5C4F-8AC2-E4191A3C93C6}">
   <dimension ref="A1:E126"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A95" workbookViewId="0">
-      <selection activeCell="C113" sqref="C113"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7:E7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.95"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="3" max="3" width="87.875" customWidth="1"/>
-    <col min="4" max="4" width="18.375" customWidth="1"/>
+    <col min="3" max="3" width="87.83203125" customWidth="1"/>
+    <col min="4" max="4" width="18.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="15.75">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2463,7 +2453,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="15.75">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -2480,7 +2470,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="15.75">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
         <v>2</v>
       </c>
@@ -2497,7 +2487,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="15.75">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" s="1">
         <v>3</v>
       </c>
@@ -2514,7 +2504,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="15.75">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" s="1">
         <v>4</v>
       </c>
@@ -2531,7 +2521,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="15.75">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" s="1">
         <v>5</v>
       </c>
@@ -2545,115 +2535,107 @@
         <v>8</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="15.75">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" s="1">
         <v>6</v>
       </c>
-      <c r="B7" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="E7" s="6" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" ht="15.75">
+      <c r="B7" s="1"/>
+      <c r="C7" s="1"/>
+      <c r="D7" s="1"/>
+      <c r="E7" s="6"/>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" s="1">
         <v>7</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="D8" s="1"/>
       <c r="E8" s="6" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="15.75">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" s="1">
         <v>8</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="D9" s="1"/>
       <c r="E9" s="6" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:5" ht="15.75">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" s="1">
         <v>9</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="E10" s="6" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="11" spans="1:5" ht="15.75">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11" s="1">
         <v>10</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="D11" s="1"/>
       <c r="E11" s="6" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="12" spans="1:5" ht="15.75">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12" s="1">
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="E12" s="6" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="13" spans="1:5" ht="15.75">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13" s="1">
         <v>12</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="D13" s="1"/>
       <c r="E13" s="6" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="14" spans="1:5" ht="15.75">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14" s="1">
         <v>13</v>
       </c>
@@ -2661,1164 +2643,1164 @@
       <c r="C14" s="4"/>
       <c r="D14" s="1"/>
     </row>
-    <row r="15" spans="1:5" ht="15.75">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15" s="1">
         <v>14</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="D15" s="1"/>
     </row>
-    <row r="16" spans="1:5" ht="15.75">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A16" s="1">
         <v>15</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="C16" s="4" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="D16" s="1"/>
     </row>
-    <row r="17" spans="1:4" ht="15.75">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A17" s="1">
         <v>16</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="C17" s="4" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="D17" s="1"/>
     </row>
-    <row r="18" spans="1:4" ht="15.75">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A18" s="1">
         <v>17</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="C18" s="4" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="D18" s="1"/>
     </row>
-    <row r="19" spans="1:4" ht="15.75">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A19" s="1">
         <v>18</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="C19" s="4" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="D19" s="1"/>
     </row>
-    <row r="20" spans="1:4" ht="15.75">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A20" s="1">
         <v>19</v>
       </c>
       <c r="B20" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="C20" s="4" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" ht="15.75">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A21" s="1">
         <v>20</v>
       </c>
       <c r="B21" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="C21" s="4" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" ht="15.75">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A22" s="1">
         <v>21</v>
       </c>
       <c r="B22" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="C22" s="4" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" ht="15.75">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A23" s="1">
         <v>22</v>
       </c>
       <c r="B23" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="C23" s="4" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" ht="15.75">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A24" s="1">
         <v>23</v>
       </c>
       <c r="B24" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="C24" s="4" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" ht="15.75">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A25" s="1">
         <v>24</v>
       </c>
       <c r="B25" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="C25" s="4" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" ht="15.75">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A26" s="1">
         <v>25</v>
       </c>
       <c r="B26" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="C26" s="4" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" ht="15.75">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A27" s="1">
         <v>26</v>
       </c>
       <c r="B27" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="C27" s="4" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" ht="15.75">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A28" s="1">
         <v>27</v>
       </c>
       <c r="B28" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="C28" s="4" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" ht="15.75">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A29" s="1">
         <v>28</v>
       </c>
       <c r="B29" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="C29" s="4" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4" ht="15.75">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A30" s="1">
         <v>29</v>
       </c>
       <c r="B30" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="C30" s="4" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4" ht="15.75">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A31" s="1">
         <v>30</v>
       </c>
       <c r="B31" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="C31" s="4" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" ht="15.75">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A32" s="1">
         <v>31</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="C32" s="4" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3" ht="15.75">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A33" s="1">
         <v>32</v>
       </c>
       <c r="B33" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="C33" s="4" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3" ht="15.75">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A34" s="1">
         <v>33</v>
       </c>
       <c r="B34" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="C34" s="4" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="35" spans="1:3" ht="15.75">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A35" s="1">
         <v>34</v>
       </c>
       <c r="B35" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="C35" s="4" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="36" spans="1:3" ht="15.75">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A36" s="1">
         <v>35</v>
       </c>
       <c r="B36" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="C36" s="4" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="37" spans="1:3" ht="15.75">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A37" s="1">
         <v>36</v>
       </c>
       <c r="B37" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="C37" s="4" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="38" spans="1:3" ht="15.75">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A38" s="1">
         <v>37</v>
       </c>
       <c r="B38" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="C38" s="4" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="39" spans="1:3" ht="15.75">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A39" s="1">
         <v>38</v>
       </c>
       <c r="B39" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="C39" s="4" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="40" spans="1:3" ht="15.75">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A40" s="1">
         <v>39</v>
       </c>
       <c r="B40" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="C40" s="4" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="41" spans="1:3" ht="15.75">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A41" s="1">
         <v>40</v>
       </c>
       <c r="B41" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="C41" s="4" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="42" spans="1:3" ht="15.75">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A42" s="1">
         <v>41</v>
       </c>
       <c r="B42" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="C42" s="4" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="43" spans="1:3" ht="15.75">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A43" s="1">
         <v>42</v>
       </c>
       <c r="B43" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="C43" s="4" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="44" spans="1:3" ht="15.75">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A44" s="1">
         <v>43</v>
       </c>
       <c r="B44" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="C44" s="4" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="45" spans="1:3" ht="15.75">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A45" s="1">
         <v>44</v>
       </c>
       <c r="B45" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="C45" s="4" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="46" spans="1:3" ht="15.75">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A46" s="1">
         <v>45</v>
       </c>
       <c r="B46" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="C46" s="4" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="47" spans="1:3" ht="15.75">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A47" s="1">
         <v>46</v>
       </c>
       <c r="B47" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="C47" s="4" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="48" spans="1:3" ht="15.75">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A48" s="1">
         <v>47</v>
       </c>
       <c r="B48" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="C48" s="4" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="49" spans="1:5" ht="15.75">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A49" s="1">
         <v>48</v>
       </c>
       <c r="B49" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="C49" s="4" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="50" spans="1:5" ht="15.75">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A50" s="1">
         <v>49</v>
       </c>
       <c r="B50" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="C50" s="4" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="51" spans="1:5" ht="15.75">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A51" s="1">
         <v>50</v>
       </c>
       <c r="B51" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="C51" s="4" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="52" spans="1:5" ht="15.75">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A52" s="1">
         <v>51</v>
       </c>
       <c r="B52" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="C52" s="4" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="53" spans="1:5" ht="15.75">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A53" s="1">
         <v>52</v>
       </c>
       <c r="B53" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="C53" s="4" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="54" spans="1:5" ht="15.75">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A54" s="1">
         <v>53</v>
       </c>
       <c r="B54" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="C54" s="4" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="55" spans="1:5" ht="15.75">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A55" s="1">
         <v>54</v>
       </c>
       <c r="B55" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="C55" s="4" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="56" spans="1:5" ht="15.75">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A56" s="1">
         <v>55</v>
       </c>
       <c r="B56" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="C56" s="4" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="57" spans="1:5" ht="15.75">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A57" s="1">
         <v>56</v>
       </c>
       <c r="B57" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="C57" s="4" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="58" spans="1:5" ht="15.75">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A58" s="1">
         <v>57</v>
       </c>
       <c r="B58" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="C58" s="4" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="59" spans="1:5" ht="15.75">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A59" s="1">
         <v>58</v>
       </c>
       <c r="B59" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="C59" s="4" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="60" spans="1:5" ht="15.75">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A60" s="1">
         <v>59</v>
       </c>
       <c r="B60" s="8" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="C60" s="4" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="61" spans="1:5" ht="15.75">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A61" s="1">
         <v>60</v>
       </c>
       <c r="B61" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="C61" s="4" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="E61" s="10" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="62" spans="1:5" ht="15.75">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A62" s="1">
         <v>61</v>
       </c>
       <c r="B62" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="C62" s="4" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="63" spans="1:5" ht="15.75">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A63" s="1">
         <v>62</v>
       </c>
       <c r="B63" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="64" spans="1:5" ht="15.75">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A64" s="1">
         <v>63</v>
       </c>
       <c r="B64" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="C64" s="4" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="E64" s="10" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="65" spans="1:3" ht="15.75">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A65" s="1">
         <v>64</v>
       </c>
       <c r="B65" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="C65" s="4" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="66" spans="1:3" ht="15.75">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A66" s="1">
         <v>65</v>
       </c>
       <c r="B66" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="C66" s="4" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="67" spans="1:3" ht="15.75">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A67" s="1">
         <v>66</v>
       </c>
       <c r="B67" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="C67" s="4" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="68" spans="1:3" ht="15.75">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A68" s="1">
         <v>67</v>
       </c>
       <c r="B68" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="C68" s="4" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="69" spans="1:3" ht="15.75">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A69" s="1">
         <v>68</v>
       </c>
       <c r="B69" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="C69" s="4" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="70" spans="1:3" ht="15.75">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A70" s="1">
         <v>69</v>
       </c>
       <c r="B70" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="C70" s="4" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="71" spans="1:3" ht="15.75">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A71" s="1">
         <v>70</v>
       </c>
       <c r="B71" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="C71" s="4" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="72" spans="1:3" ht="15.75">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="72" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A72" s="1">
         <v>71</v>
       </c>
       <c r="B72" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="C72" s="4" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="73" spans="1:3" ht="15.75">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="73" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A73" s="1">
         <v>72</v>
       </c>
       <c r="B73" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="C73" s="4" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="74" spans="1:3" ht="15.75">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="74" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A74" s="1">
         <v>73</v>
       </c>
       <c r="B74" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="75" spans="1:3" ht="15.75">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="75" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A75" s="1">
         <v>74</v>
       </c>
       <c r="B75" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="C75" s="4" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="76" spans="1:3" ht="15.75">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="76" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A76" s="1">
         <v>75</v>
       </c>
       <c r="B76" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="C76" s="4" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="77" spans="1:3" ht="15.75">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="77" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A77" s="1">
         <v>76</v>
       </c>
       <c r="B77" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="C77" s="4" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="78" spans="1:3" ht="15.75">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="78" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A78" s="1">
         <v>77</v>
       </c>
       <c r="B78" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="C78" s="4" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="79" spans="1:3" ht="15.75">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="79" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A79" s="1">
         <v>78</v>
       </c>
       <c r="B79" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="C79" s="4" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="80" spans="1:3" ht="15.75">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="80" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A80" s="1">
         <v>79</v>
       </c>
       <c r="B80" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="C80" s="4" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="81" spans="1:3" ht="15.75">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="81" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A81" s="1">
         <v>80</v>
       </c>
       <c r="B81" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="C81" s="4" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="82" spans="1:3" ht="15.75">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="82" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A82" s="1">
         <v>81</v>
       </c>
       <c r="B82" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="C82" s="4" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="83" spans="1:3" ht="15.75">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="83" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A83" s="1">
         <v>82</v>
       </c>
       <c r="B83" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="C83" s="4" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="84" spans="1:3" ht="15.75">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="84" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A84" s="1">
         <v>83</v>
       </c>
       <c r="B84" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="C84" s="4" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="85" spans="1:3" ht="15.75">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="85" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A85" s="1">
         <v>84</v>
       </c>
       <c r="B85" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="C85" s="4" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="86" spans="1:3" ht="15.75">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="86" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A86" s="1">
         <v>85</v>
       </c>
       <c r="B86" s="8" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="C86" s="4" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="87" spans="1:3" ht="15.75">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="87" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A87" s="1">
         <v>86</v>
       </c>
       <c r="B87" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="C87" s="4" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="88" spans="1:3" ht="15.75">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="88" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A88" s="1">
         <v>87</v>
       </c>
       <c r="B88" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="C88" s="4" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="89" spans="1:3" ht="15.75">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="89" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A89" s="1">
         <v>88</v>
       </c>
       <c r="B89" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="C89" s="4" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="90" spans="1:3" ht="15.75">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="90" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A90" s="1">
         <v>89</v>
       </c>
       <c r="B90" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="C90" s="4" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="91" spans="1:3" ht="15.75">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="91" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A91" s="1">
         <v>90</v>
       </c>
       <c r="B91" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="C91" s="4" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="92" spans="1:3" ht="15.75">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="92" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A92" s="1">
         <v>91</v>
       </c>
       <c r="B92" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="C92" s="4" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="93" spans="1:3" ht="15.75">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="93" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A93" s="1">
         <v>92</v>
       </c>
       <c r="B93" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="C93" s="4" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="94" spans="1:3" ht="15.75">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="94" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A94" s="1">
         <v>93</v>
       </c>
       <c r="B94" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="C94" s="4" t="s">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="95" spans="1:3" ht="15.75">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="95" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A95" s="1">
         <v>94</v>
       </c>
       <c r="B95" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="C95" s="4" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="96" spans="1:3" ht="15.75">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="96" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A96" s="1">
         <v>95</v>
       </c>
       <c r="B96" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="C96" s="4" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="97" spans="1:5" ht="15.75">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="97" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A97" s="1">
         <v>96</v>
       </c>
       <c r="B97" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="C97" s="4" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="98" spans="1:5" ht="15.75">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="98" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A98" s="1">
         <v>97</v>
       </c>
       <c r="B98" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="C98" s="4" t="s">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="99" spans="1:5" ht="15.75">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="99" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A99" s="1">
         <v>98</v>
       </c>
       <c r="B99" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="C99" s="4" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="100" spans="1:5" ht="15.75">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="100" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A100" s="1">
         <v>99</v>
       </c>
       <c r="B100" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
       <c r="C100" s="4" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="101" spans="1:5" ht="15.75">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="101" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A101" s="1">
         <v>100</v>
       </c>
       <c r="B101" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="C101" s="4" t="s">
-        <v>207</v>
-      </c>
-    </row>
-    <row r="102" spans="1:5" ht="15.75">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="102" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A102" s="1">
         <v>101</v>
       </c>
       <c r="B102" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="C102" s="4" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="103" spans="1:5" ht="15.75">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="103" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A103" s="1">
         <v>102</v>
       </c>
       <c r="B103" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
       <c r="C103" s="4" t="s">
-        <v>211</v>
-      </c>
-    </row>
-    <row r="104" spans="1:5" ht="15.75">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="104" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A104" s="1">
         <v>103</v>
       </c>
       <c r="B104" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="C104" s="4" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="105" spans="1:5" ht="15.75">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="105" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A105" s="1">
         <v>104</v>
       </c>
       <c r="B105" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
       <c r="C105" s="4" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="106" spans="1:5" ht="15.75">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="106" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A106" s="1">
         <v>105</v>
       </c>
       <c r="B106" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
       <c r="C106" s="4" t="s">
-        <v>217</v>
-      </c>
-    </row>
-    <row r="107" spans="1:5" ht="15.75">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="107" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A107" s="1">
         <v>106</v>
       </c>
       <c r="B107" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
       <c r="C107" s="4" t="s">
-        <v>219</v>
-      </c>
-    </row>
-    <row r="108" spans="1:5" ht="15.75">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="108" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A108" s="1">
         <v>107</v>
       </c>
       <c r="B108" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="C108" s="4" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
       <c r="E108" s="9" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="109" spans="1:5" ht="15.75">
+    <row r="109" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A109" s="1">
         <v>108</v>
       </c>
       <c r="B109" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="C109" s="4" t="s">
-        <v>223</v>
-      </c>
-    </row>
-    <row r="110" spans="1:5" ht="15.75">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="110" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A110" s="1">
         <v>109</v>
       </c>
       <c r="B110" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
       <c r="C110" s="4" t="s">
-        <v>225</v>
-      </c>
-    </row>
-    <row r="111" spans="1:5" ht="15.75">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="111" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A111" s="1">
         <v>110</v>
       </c>
       <c r="B111" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
       <c r="C111" s="4" t="s">
-        <v>227</v>
-      </c>
-    </row>
-    <row r="112" spans="1:5" ht="15.75">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="112" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A112" s="1">
         <v>111</v>
       </c>
       <c r="B112" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
       <c r="C112" s="4" t="s">
-        <v>229</v>
-      </c>
-    </row>
-    <row r="113" spans="1:3" ht="15.75">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="113" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A113" s="1">
         <v>112</v>
       </c>
       <c r="B113" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
       <c r="C113" s="4" t="s">
-        <v>231</v>
-      </c>
-    </row>
-    <row r="114" spans="1:3" ht="15.75">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="114" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A114" s="1">
         <v>113</v>
       </c>
     </row>
-    <row r="115" spans="1:3" ht="15.75">
+    <row r="115" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A115" s="1">
         <v>114</v>
       </c>
     </row>
-    <row r="116" spans="1:3" ht="15.75">
+    <row r="116" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A116" s="1">
         <v>115</v>
       </c>
     </row>
-    <row r="117" spans="1:3" ht="15.75">
+    <row r="117" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A117" s="1">
         <v>116</v>
       </c>
     </row>
-    <row r="118" spans="1:3" ht="15.75">
+    <row r="118" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A118" s="1">
         <v>117</v>
       </c>
     </row>
-    <row r="119" spans="1:3" ht="15.75">
+    <row r="119" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A119" s="1">
         <v>118</v>
       </c>
     </row>
-    <row r="120" spans="1:3" ht="15.75">
+    <row r="120" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A120" s="1">
         <v>119</v>
       </c>
     </row>
-    <row r="121" spans="1:3" ht="15.75">
+    <row r="121" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A121" s="1">
         <v>120</v>
       </c>
     </row>
-    <row r="122" spans="1:3" ht="15.75">
+    <row r="122" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A122" s="1">
         <v>121</v>
       </c>
     </row>
-    <row r="123" spans="1:3" ht="15.75">
+    <row r="123" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A123" s="1">
         <v>122</v>
       </c>
     </row>
-    <row r="124" spans="1:3" ht="15.75">
+    <row r="124" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A124" s="1">
         <v>123</v>
       </c>
     </row>
-    <row r="125" spans="1:3" ht="15.75">
+    <row r="125" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A125" s="1">
         <v>124</v>
       </c>
     </row>
-    <row r="126" spans="1:3" ht="15.75">
+    <row r="126" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A126" s="1">
         <v>125</v>
       </c>
@@ -3942,949 +3924,949 @@
       <selection sqref="A1:C90"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
+        <v>229</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>230</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>232</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C2" s="1" t="s">
         <v>233</v>
       </c>
-      <c r="C1" s="1" t="s">
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3" s="1" t="s">
         <v>234</v>
       </c>
-    </row>
-    <row r="2" spans="1:3">
-      <c r="A2" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="B2" s="1" t="s">
+      <c r="B3" s="1" t="s">
         <v>235</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="C3" s="1" t="s">
         <v>236</v>
       </c>
     </row>
-    <row r="3" spans="1:3">
-      <c r="A3" s="1" t="s">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A4" s="1" t="s">
         <v>237</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B4" s="1" t="s">
         <v>238</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="C4" s="1" t="s">
         <v>239</v>
       </c>
     </row>
-    <row r="4" spans="1:3">
-      <c r="A4" s="1" t="s">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A5" s="1" t="s">
         <v>240</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="B5" s="1" t="s">
         <v>241</v>
       </c>
-      <c r="C4" s="1" t="s">
+      <c r="C5" s="1" t="s">
         <v>242</v>
       </c>
     </row>
-    <row r="5" spans="1:3">
-      <c r="A5" s="1" t="s">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6" s="1" t="s">
         <v>243</v>
       </c>
-      <c r="B5" s="1" t="s">
+      <c r="B6" s="1" t="s">
         <v>244</v>
       </c>
-      <c r="C5" s="1" t="s">
+      <c r="C6" s="1" t="s">
         <v>245</v>
       </c>
     </row>
-    <row r="6" spans="1:3">
-      <c r="A6" s="1" t="s">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A7" s="1" t="s">
         <v>246</v>
       </c>
-      <c r="B6" s="1" t="s">
+      <c r="B7" s="1" t="s">
         <v>247</v>
       </c>
-      <c r="C6" s="1" t="s">
+      <c r="C7" s="1" t="s">
         <v>248</v>
       </c>
     </row>
-    <row r="7" spans="1:3">
-      <c r="A7" s="1" t="s">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A8" s="1" t="s">
         <v>249</v>
       </c>
-      <c r="B7" s="1" t="s">
+      <c r="B8" s="1" t="s">
         <v>250</v>
       </c>
-      <c r="C7" s="1" t="s">
+      <c r="C8" s="1" t="s">
         <v>251</v>
       </c>
     </row>
-    <row r="8" spans="1:3">
-      <c r="A8" s="1" t="s">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A9" s="1" t="s">
         <v>252</v>
       </c>
-      <c r="B8" s="1" t="s">
+      <c r="B9" s="1" t="s">
         <v>253</v>
       </c>
-      <c r="C8" s="1" t="s">
+      <c r="C9" s="1" t="s">
         <v>254</v>
       </c>
     </row>
-    <row r="9" spans="1:3">
-      <c r="A9" s="1" t="s">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A10" s="1" t="s">
         <v>255</v>
       </c>
-      <c r="B9" s="1" t="s">
+      <c r="B10" s="1" t="s">
         <v>256</v>
       </c>
-      <c r="C9" s="1" t="s">
+      <c r="C10" s="1" t="s">
         <v>257</v>
       </c>
     </row>
-    <row r="10" spans="1:3">
-      <c r="A10" s="1" t="s">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A11" s="1" t="s">
         <v>258</v>
       </c>
-      <c r="B10" s="1" t="s">
+      <c r="B11" s="1" t="s">
         <v>259</v>
       </c>
-      <c r="C10" s="1" t="s">
+      <c r="C11" s="1" t="s">
         <v>260</v>
       </c>
     </row>
-    <row r="11" spans="1:3">
-      <c r="A11" s="1" t="s">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A12" s="1" t="s">
         <v>261</v>
       </c>
-      <c r="B11" s="1" t="s">
+      <c r="B12" s="1" t="s">
         <v>262</v>
       </c>
-      <c r="C11" s="1" t="s">
+      <c r="C12" s="1" t="s">
         <v>263</v>
       </c>
     </row>
-    <row r="12" spans="1:3">
-      <c r="A12" s="1" t="s">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A13" s="1" t="s">
         <v>264</v>
       </c>
-      <c r="B12" s="1" t="s">
+      <c r="B13" s="1" t="s">
         <v>265</v>
       </c>
-      <c r="C12" s="1" t="s">
+      <c r="C13" s="1" t="s">
         <v>266</v>
       </c>
     </row>
-    <row r="13" spans="1:3">
-      <c r="A13" s="1" t="s">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A14" s="1" t="s">
         <v>267</v>
       </c>
-      <c r="B13" s="1" t="s">
+      <c r="B14" s="1" t="s">
         <v>268</v>
       </c>
-      <c r="C13" s="1" t="s">
+      <c r="C14" s="1" t="s">
         <v>269</v>
       </c>
     </row>
-    <row r="14" spans="1:3">
-      <c r="A14" s="1" t="s">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A15" s="1" t="s">
         <v>270</v>
       </c>
-      <c r="B14" s="1" t="s">
+      <c r="B15" s="1" t="s">
         <v>271</v>
       </c>
-      <c r="C14" s="1" t="s">
+      <c r="C15" s="1" t="s">
         <v>272</v>
       </c>
     </row>
-    <row r="15" spans="1:3">
-      <c r="A15" s="1" t="s">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A16" s="1" t="s">
         <v>273</v>
       </c>
-      <c r="B15" s="1" t="s">
+      <c r="B16" s="1" t="s">
         <v>274</v>
       </c>
-      <c r="C15" s="1" t="s">
+      <c r="C16" s="1" t="s">
         <v>275</v>
       </c>
     </row>
-    <row r="16" spans="1:3">
-      <c r="A16" s="1" t="s">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A17" s="1" t="s">
         <v>276</v>
       </c>
-      <c r="B16" s="1" t="s">
+      <c r="B17" s="1" t="s">
         <v>277</v>
       </c>
-      <c r="C16" s="1" t="s">
+      <c r="C17" s="1" t="s">
         <v>278</v>
       </c>
     </row>
-    <row r="17" spans="1:3">
-      <c r="A17" s="1" t="s">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A18" s="1" t="s">
         <v>279</v>
       </c>
-      <c r="B17" s="1" t="s">
+      <c r="B18" s="2" t="s">
         <v>280</v>
       </c>
-      <c r="C17" s="1" t="s">
+      <c r="C18" s="1" t="s">
         <v>281</v>
       </c>
     </row>
-    <row r="18" spans="1:3">
-      <c r="A18" s="1" t="s">
-        <v>282</v>
-      </c>
-      <c r="B18" s="2" t="s">
-        <v>283</v>
-      </c>
-      <c r="C18" s="1" t="s">
-        <v>284</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A19" s="1"/>
       <c r="B19" s="1"/>
       <c r="C19" s="1"/>
     </row>
-    <row r="20" spans="1:3">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
+        <v>282</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>283</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A21" s="1" t="s">
         <v>285</v>
       </c>
-      <c r="B20" s="2" t="s">
+      <c r="B21" s="1" t="s">
         <v>286</v>
       </c>
-      <c r="C20" s="1" t="s">
+      <c r="C21" s="1" t="s">
         <v>287</v>
       </c>
     </row>
-    <row r="21" spans="1:3">
-      <c r="A21" s="1" t="s">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A22" s="1" t="s">
         <v>288</v>
       </c>
-      <c r="B21" s="1" t="s">
+      <c r="B22" s="1" t="s">
         <v>289</v>
       </c>
-      <c r="C21" s="1" t="s">
+      <c r="C22" s="1" t="s">
         <v>290</v>
       </c>
     </row>
-    <row r="22" spans="1:3">
-      <c r="A22" s="1" t="s">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A23" s="1" t="s">
         <v>291</v>
       </c>
-      <c r="B22" s="1" t="s">
+      <c r="B23" s="1" t="s">
         <v>292</v>
       </c>
-      <c r="C22" s="1" t="s">
+      <c r="C23" s="1" t="s">
         <v>293</v>
       </c>
     </row>
-    <row r="23" spans="1:3">
-      <c r="A23" s="1" t="s">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A24" s="1" t="s">
         <v>294</v>
       </c>
-      <c r="B23" s="1" t="s">
+      <c r="B24" s="1" t="s">
         <v>295</v>
       </c>
-      <c r="C23" s="1" t="s">
+      <c r="C24" s="1" t="s">
         <v>296</v>
       </c>
     </row>
-    <row r="24" spans="1:3">
-      <c r="A24" s="1" t="s">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A25" s="1" t="s">
         <v>297</v>
       </c>
-      <c r="B24" s="1" t="s">
+      <c r="B25" s="1" t="s">
         <v>298</v>
       </c>
-      <c r="C24" s="1" t="s">
+      <c r="C25" s="1" t="s">
         <v>299</v>
       </c>
     </row>
-    <row r="25" spans="1:3">
-      <c r="A25" s="1" t="s">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A26" s="1" t="s">
         <v>300</v>
       </c>
-      <c r="B25" s="1" t="s">
+      <c r="B26" s="1" t="s">
         <v>301</v>
       </c>
-      <c r="C25" s="1" t="s">
+      <c r="C26" s="1" t="s">
         <v>302</v>
       </c>
     </row>
-    <row r="26" spans="1:3">
-      <c r="A26" s="1" t="s">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A27" s="1" t="s">
         <v>303</v>
       </c>
-      <c r="B26" s="1" t="s">
+      <c r="B27" s="1" t="s">
         <v>304</v>
       </c>
-      <c r="C26" s="1" t="s">
+      <c r="C27" s="1" t="s">
         <v>305</v>
       </c>
     </row>
-    <row r="27" spans="1:3">
-      <c r="A27" s="1" t="s">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A28" s="1" t="s">
         <v>306</v>
       </c>
-      <c r="B27" s="1" t="s">
+      <c r="B28" s="1" t="s">
         <v>307</v>
       </c>
-      <c r="C27" s="1" t="s">
+      <c r="C28" s="1" t="s">
         <v>308</v>
       </c>
     </row>
-    <row r="28" spans="1:3">
-      <c r="A28" s="1" t="s">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A29" s="1" t="s">
         <v>309</v>
       </c>
-      <c r="B28" s="1" t="s">
+      <c r="B29" s="1" t="s">
         <v>310</v>
       </c>
-      <c r="C28" s="1" t="s">
+      <c r="C29" s="1" t="s">
         <v>311</v>
       </c>
     </row>
-    <row r="29" spans="1:3">
-      <c r="A29" s="1" t="s">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A30" s="1" t="s">
         <v>312</v>
       </c>
-      <c r="B29" s="1" t="s">
+      <c r="B30" s="1" t="s">
         <v>313</v>
       </c>
-      <c r="C29" s="1" t="s">
+      <c r="C30" s="1" t="s">
         <v>314</v>
       </c>
     </row>
-    <row r="30" spans="1:3">
-      <c r="A30" s="1" t="s">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A31" s="1" t="s">
         <v>315</v>
       </c>
-      <c r="B30" s="1" t="s">
+      <c r="B31" s="1" t="s">
         <v>316</v>
       </c>
-      <c r="C30" s="1" t="s">
+      <c r="C31" s="1" t="s">
         <v>317</v>
       </c>
     </row>
-    <row r="31" spans="1:3">
-      <c r="A31" s="1" t="s">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A32" s="1" t="s">
         <v>318</v>
       </c>
-      <c r="B31" s="1" t="s">
+      <c r="B32" s="1" t="s">
         <v>319</v>
       </c>
-      <c r="C31" s="1" t="s">
+      <c r="C32" s="1" t="s">
         <v>320</v>
       </c>
     </row>
-    <row r="32" spans="1:3">
-      <c r="A32" s="1" t="s">
-        <v>321</v>
-      </c>
-      <c r="B32" s="1" t="s">
-        <v>322</v>
-      </c>
-      <c r="C32" s="1" t="s">
-        <v>323</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A33" s="1"/>
       <c r="B33" s="3"/>
       <c r="C33" s="1"/>
     </row>
-    <row r="34" spans="1:3">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A34" s="1" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
       <c r="B34" s="2" t="s">
+        <v>321</v>
+      </c>
+      <c r="C34" s="1" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A35" s="1" t="s">
+        <v>267</v>
+      </c>
+      <c r="B35" s="2" t="s">
+        <v>323</v>
+      </c>
+      <c r="C35" s="1" t="s">
         <v>324</v>
       </c>
-      <c r="C34" s="1" t="s">
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A36" s="1" t="s">
         <v>325</v>
       </c>
-    </row>
-    <row r="35" spans="1:3">
-      <c r="A35" s="1" t="s">
-        <v>270</v>
-      </c>
-      <c r="B35" s="2" t="s">
+      <c r="B36" s="1" t="s">
         <v>326</v>
       </c>
-      <c r="C35" s="1" t="s">
+      <c r="C36" s="1" t="s">
         <v>327</v>
       </c>
     </row>
-    <row r="36" spans="1:3">
-      <c r="A36" s="1" t="s">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A37" s="1" t="s">
         <v>328</v>
       </c>
-      <c r="B36" s="1" t="s">
+      <c r="B37" s="2" t="s">
         <v>329</v>
       </c>
-      <c r="C36" s="1" t="s">
+      <c r="C37" s="1" t="s">
         <v>330</v>
       </c>
     </row>
-    <row r="37" spans="1:3">
-      <c r="A37" s="1" t="s">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A38" s="1" t="s">
         <v>331</v>
       </c>
-      <c r="B37" s="2" t="s">
+      <c r="B38" s="1" t="s">
         <v>332</v>
       </c>
-      <c r="C37" s="1" t="s">
+      <c r="C38" s="1" t="s">
         <v>333</v>
       </c>
     </row>
-    <row r="38" spans="1:3">
-      <c r="A38" s="1" t="s">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A39" s="1" t="s">
         <v>334</v>
       </c>
-      <c r="B38" s="1" t="s">
+      <c r="B39" s="1" t="s">
         <v>335</v>
       </c>
-      <c r="C38" s="1" t="s">
+      <c r="C39" s="1" t="s">
         <v>336</v>
       </c>
     </row>
-    <row r="39" spans="1:3">
-      <c r="A39" s="1" t="s">
-        <v>337</v>
-      </c>
-      <c r="B39" s="1" t="s">
-        <v>338</v>
-      </c>
-      <c r="C39" s="1" t="s">
-        <v>339</v>
-      </c>
-    </row>
-    <row r="40" spans="1:3">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A40" s="1"/>
       <c r="B40" s="1"/>
       <c r="C40" s="1"/>
     </row>
-    <row r="41" spans="1:3">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A41" s="1" t="s">
-        <v>340</v>
+        <v>337</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>341</v>
+        <v>338</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>342</v>
-      </c>
-    </row>
-    <row r="42" spans="1:3">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A42" s="1"/>
       <c r="B42" s="1"/>
       <c r="C42" s="1"/>
     </row>
-    <row r="43" spans="1:3">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A43" s="1" t="s">
+        <v>340</v>
+      </c>
+      <c r="B43" s="1" t="s">
+        <v>341</v>
+      </c>
+      <c r="C43" s="1" t="s">
+        <v>342</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A44" s="1" t="s">
         <v>343</v>
       </c>
-      <c r="B43" s="1" t="s">
+      <c r="B44" s="1" t="s">
         <v>344</v>
       </c>
-      <c r="C43" s="1" t="s">
+      <c r="C44" s="1" t="s">
         <v>345</v>
       </c>
     </row>
-    <row r="44" spans="1:3">
-      <c r="A44" s="1" t="s">
+    <row r="45" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A45" s="1" t="s">
         <v>346</v>
       </c>
-      <c r="B44" s="1" t="s">
+      <c r="B45" s="1" t="s">
         <v>347</v>
       </c>
-      <c r="C44" s="1" t="s">
+      <c r="C45" s="1" t="s">
         <v>348</v>
       </c>
     </row>
-    <row r="45" spans="1:3">
-      <c r="A45" s="1" t="s">
+    <row r="46" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A46" s="1" t="s">
         <v>349</v>
       </c>
-      <c r="B45" s="1" t="s">
+      <c r="B46" s="2" t="s">
         <v>350</v>
       </c>
-      <c r="C45" s="1" t="s">
+      <c r="C46" s="1" t="s">
         <v>351</v>
       </c>
     </row>
-    <row r="46" spans="1:3">
-      <c r="A46" s="1" t="s">
+    <row r="47" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A47" s="1" t="s">
         <v>352</v>
       </c>
-      <c r="B46" s="2" t="s">
+      <c r="B47" s="1" t="s">
+        <v>352</v>
+      </c>
+      <c r="C47" s="1" t="s">
         <v>353</v>
       </c>
-      <c r="C46" s="1" t="s">
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A48" s="1" t="s">
         <v>354</v>
       </c>
-    </row>
-    <row r="47" spans="1:3">
-      <c r="A47" s="1" t="s">
+      <c r="B48" s="1" t="s">
         <v>355</v>
       </c>
-      <c r="B47" s="1" t="s">
-        <v>355</v>
-      </c>
-      <c r="C47" s="1" t="s">
+      <c r="C48" s="1" t="s">
         <v>356</v>
       </c>
     </row>
-    <row r="48" spans="1:3">
-      <c r="A48" s="1" t="s">
+    <row r="49" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A49" s="1" t="s">
         <v>357</v>
       </c>
-      <c r="B48" s="1" t="s">
+      <c r="B49" s="1" t="s">
         <v>358</v>
       </c>
-      <c r="C48" s="1" t="s">
+      <c r="C49" s="1" t="s">
         <v>359</v>
       </c>
     </row>
-    <row r="49" spans="1:3">
-      <c r="A49" s="1" t="s">
+    <row r="50" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A50" s="1" t="s">
         <v>360</v>
       </c>
-      <c r="B49" s="1" t="s">
+      <c r="B50" s="1" t="s">
         <v>361</v>
       </c>
-      <c r="C49" s="1" t="s">
+      <c r="C50" s="1" t="s">
         <v>362</v>
       </c>
     </row>
-    <row r="50" spans="1:3">
-      <c r="A50" s="1" t="s">
+    <row r="51" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A51" s="1" t="s">
         <v>363</v>
       </c>
-      <c r="B50" s="1" t="s">
+      <c r="B51" s="1" t="s">
         <v>364</v>
       </c>
-      <c r="C50" s="1" t="s">
+      <c r="C51" s="1" t="s">
         <v>365</v>
       </c>
     </row>
-    <row r="51" spans="1:3">
-      <c r="A51" s="1" t="s">
+    <row r="52" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A52" s="1" t="s">
         <v>366</v>
       </c>
-      <c r="B51" s="1" t="s">
+      <c r="B52" s="1" t="s">
         <v>367</v>
       </c>
-      <c r="C51" s="1" t="s">
+      <c r="C52" s="1" t="s">
         <v>368</v>
       </c>
     </row>
-    <row r="52" spans="1:3">
-      <c r="A52" s="1" t="s">
+    <row r="53" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A53" s="1" t="s">
         <v>369</v>
       </c>
-      <c r="B52" s="1" t="s">
+      <c r="B53" s="1" t="s">
         <v>370</v>
       </c>
-      <c r="C52" s="1" t="s">
+      <c r="C53" s="1" t="s">
         <v>371</v>
       </c>
     </row>
-    <row r="53" spans="1:3">
-      <c r="A53" s="1" t="s">
+    <row r="54" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A54" s="1" t="s">
         <v>372</v>
       </c>
-      <c r="B53" s="1" t="s">
+      <c r="B54" s="1" t="s">
         <v>373</v>
       </c>
-      <c r="C53" s="1" t="s">
+      <c r="C54" s="1" t="s">
         <v>374</v>
       </c>
     </row>
-    <row r="54" spans="1:3">
-      <c r="A54" s="1" t="s">
+    <row r="55" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A55" s="1" t="s">
         <v>375</v>
       </c>
-      <c r="B54" s="1" t="s">
+      <c r="B55" s="1" t="s">
         <v>376</v>
       </c>
-      <c r="C54" s="1" t="s">
+      <c r="C55" s="1" t="s">
         <v>377</v>
       </c>
     </row>
-    <row r="55" spans="1:3">
-      <c r="A55" s="1" t="s">
+    <row r="56" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A56" s="1" t="s">
         <v>378</v>
       </c>
-      <c r="B55" s="1" t="s">
+      <c r="B56" s="2" t="s">
         <v>379</v>
       </c>
-      <c r="C55" s="1" t="s">
+      <c r="C56" s="1" t="s">
         <v>380</v>
       </c>
     </row>
-    <row r="56" spans="1:3">
-      <c r="A56" s="1" t="s">
+    <row r="58" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A58" s="1" t="s">
         <v>381</v>
       </c>
-      <c r="B56" s="2" t="s">
+      <c r="B58" s="1" t="s">
         <v>382</v>
       </c>
-      <c r="C56" s="1" t="s">
+      <c r="C58" s="1" t="s">
         <v>383</v>
       </c>
     </row>
-    <row r="58" spans="1:3">
-      <c r="A58" s="1" t="s">
+    <row r="59" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A59" s="1" t="s">
         <v>384</v>
       </c>
-      <c r="B58" s="1" t="s">
+      <c r="B59" s="1" t="s">
         <v>385</v>
       </c>
-      <c r="C58" s="1" t="s">
+      <c r="C59" s="1" t="s">
         <v>386</v>
       </c>
     </row>
-    <row r="59" spans="1:3">
-      <c r="A59" s="1" t="s">
+    <row r="60" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A60" s="1" t="s">
         <v>387</v>
       </c>
-      <c r="B59" s="1" t="s">
+      <c r="B60" s="1" t="s">
         <v>388</v>
       </c>
-      <c r="C59" s="1" t="s">
+      <c r="C60" s="1" t="s">
         <v>389</v>
       </c>
     </row>
-    <row r="60" spans="1:3">
-      <c r="A60" s="1" t="s">
+    <row r="61" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A61" s="1" t="s">
         <v>390</v>
       </c>
-      <c r="B60" s="1" t="s">
+      <c r="B61" s="1" t="s">
         <v>391</v>
       </c>
-      <c r="C60" s="1" t="s">
+      <c r="C61" s="1" t="s">
         <v>392</v>
       </c>
     </row>
-    <row r="61" spans="1:3">
-      <c r="A61" s="1" t="s">
+    <row r="62" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A62" s="1" t="s">
         <v>393</v>
       </c>
-      <c r="B61" s="1" t="s">
+      <c r="B62" s="1" t="s">
         <v>394</v>
       </c>
-      <c r="C61" s="1" t="s">
+      <c r="C62" s="1" t="s">
         <v>395</v>
       </c>
     </row>
-    <row r="62" spans="1:3">
-      <c r="A62" s="1" t="s">
+    <row r="63" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A63" s="1" t="s">
         <v>396</v>
       </c>
-      <c r="B62" s="1" t="s">
+      <c r="B63" s="1" t="s">
         <v>397</v>
       </c>
-      <c r="C62" s="1" t="s">
+      <c r="C63" s="1" t="s">
         <v>398</v>
       </c>
     </row>
-    <row r="63" spans="1:3">
-      <c r="A63" s="1" t="s">
+    <row r="64" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A64" s="1" t="s">
         <v>399</v>
       </c>
-      <c r="B63" s="1" t="s">
+      <c r="B64" s="1" t="s">
         <v>400</v>
       </c>
-      <c r="C63" s="1" t="s">
+      <c r="C64" s="1" t="s">
         <v>401</v>
       </c>
     </row>
-    <row r="64" spans="1:3">
-      <c r="A64" s="1" t="s">
+    <row r="65" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A65" s="1" t="s">
         <v>402</v>
       </c>
-      <c r="B64" s="1" t="s">
+      <c r="B65" s="1" t="s">
         <v>403</v>
       </c>
-      <c r="C64" s="1" t="s">
+      <c r="C65" s="1" t="s">
         <v>404</v>
       </c>
     </row>
-    <row r="65" spans="1:3">
-      <c r="A65" s="1" t="s">
+    <row r="66" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A66" s="1" t="s">
         <v>405</v>
       </c>
-      <c r="B65" s="1" t="s">
+      <c r="B66" s="1" t="s">
         <v>406</v>
       </c>
-      <c r="C65" s="1" t="s">
+      <c r="C66" s="1" t="s">
         <v>407</v>
       </c>
     </row>
-    <row r="66" spans="1:3">
-      <c r="A66" s="1" t="s">
+    <row r="67" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A67" s="1" t="s">
         <v>408</v>
       </c>
-      <c r="B66" s="1" t="s">
+      <c r="B67" s="1" t="s">
         <v>409</v>
       </c>
-      <c r="C66" s="1" t="s">
+      <c r="C67" s="1" t="s">
         <v>410</v>
       </c>
     </row>
-    <row r="67" spans="1:3">
-      <c r="A67" s="1" t="s">
+    <row r="68" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A68" s="1" t="s">
         <v>411</v>
       </c>
-      <c r="B67" s="1" t="s">
+      <c r="B68" s="1" t="s">
         <v>412</v>
       </c>
-      <c r="C67" s="1" t="s">
+      <c r="C68" s="1" t="s">
         <v>413</v>
       </c>
     </row>
-    <row r="68" spans="1:3">
-      <c r="A68" s="1" t="s">
+    <row r="69" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A69" s="1" t="s">
         <v>414</v>
       </c>
-      <c r="B68" s="1" t="s">
+      <c r="B69" s="1" t="s">
         <v>415</v>
       </c>
-      <c r="C68" s="1" t="s">
+      <c r="C69" s="1" t="s">
         <v>416</v>
       </c>
     </row>
-    <row r="69" spans="1:3">
-      <c r="A69" s="1" t="s">
+    <row r="70" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A70" s="1" t="s">
         <v>417</v>
       </c>
-      <c r="B69" s="1" t="s">
+      <c r="B70" s="1" t="s">
         <v>418</v>
       </c>
-      <c r="C69" s="1" t="s">
+      <c r="C70" s="1" t="s">
         <v>419</v>
       </c>
     </row>
-    <row r="70" spans="1:3">
-      <c r="A70" s="1" t="s">
+    <row r="71" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A71" s="1" t="s">
         <v>420</v>
       </c>
-      <c r="B70" s="1" t="s">
+      <c r="B71" s="1" t="s">
         <v>421</v>
       </c>
-      <c r="C70" s="1" t="s">
+      <c r="C71" s="1" t="s">
         <v>422</v>
       </c>
     </row>
-    <row r="71" spans="1:3">
-      <c r="A71" s="1" t="s">
+    <row r="72" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A72" s="1" t="s">
         <v>423</v>
       </c>
-      <c r="B71" s="1" t="s">
+      <c r="B72" s="1" t="s">
         <v>424</v>
       </c>
-      <c r="C71" s="1" t="s">
+      <c r="C72" s="1" t="s">
         <v>425</v>
       </c>
     </row>
-    <row r="72" spans="1:3">
-      <c r="A72" s="1" t="s">
-        <v>426</v>
-      </c>
-      <c r="B72" s="1" t="s">
-        <v>427</v>
-      </c>
-      <c r="C72" s="1" t="s">
-        <v>428</v>
-      </c>
-    </row>
-    <row r="73" spans="1:3">
+    <row r="73" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A73" s="1"/>
       <c r="B73" s="1"/>
       <c r="C73" s="1"/>
     </row>
-    <row r="74" spans="1:3">
+    <row r="74" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A74" s="1" t="s">
+        <v>426</v>
+      </c>
+      <c r="B74" s="1" t="s">
+        <v>427</v>
+      </c>
+      <c r="C74" s="1" t="s">
+        <v>428</v>
+      </c>
+    </row>
+    <row r="75" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A75" s="1" t="s">
         <v>429</v>
       </c>
-      <c r="B74" s="1" t="s">
+      <c r="B75" s="1" t="s">
         <v>430</v>
       </c>
-      <c r="C74" s="1" t="s">
+      <c r="C75" s="1" t="s">
         <v>431</v>
       </c>
     </row>
-    <row r="75" spans="1:3">
-      <c r="A75" s="1" t="s">
+    <row r="76" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A76" s="1" t="s">
         <v>432</v>
       </c>
-      <c r="B75" s="1" t="s">
+      <c r="B76" s="1" t="s">
         <v>433</v>
       </c>
-      <c r="C75" s="1" t="s">
+      <c r="C76" s="1" t="s">
         <v>434</v>
       </c>
     </row>
-    <row r="76" spans="1:3">
-      <c r="A76" s="1" t="s">
+    <row r="77" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A77" s="1" t="s">
         <v>435</v>
       </c>
-      <c r="B76" s="1" t="s">
+      <c r="B77" s="1" t="s">
         <v>436</v>
       </c>
-      <c r="C76" s="1" t="s">
+      <c r="C77" s="1" t="s">
         <v>437</v>
       </c>
     </row>
-    <row r="77" spans="1:3">
-      <c r="A77" s="1" t="s">
+    <row r="78" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A78" s="1" t="s">
+        <v>426</v>
+      </c>
+      <c r="B78" s="1" t="s">
         <v>438</v>
       </c>
-      <c r="B77" s="1" t="s">
+      <c r="C78" s="1" t="s">
+        <v>428</v>
+      </c>
+    </row>
+    <row r="79" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A79" s="1" t="s">
         <v>439</v>
       </c>
-      <c r="C77" s="1" t="s">
+      <c r="B79" s="1" t="s">
         <v>440</v>
       </c>
-    </row>
-    <row r="78" spans="1:3">
-      <c r="A78" s="1" t="s">
-        <v>429</v>
-      </c>
-      <c r="B78" s="1" t="s">
+      <c r="C79" s="1" t="s">
         <v>441</v>
       </c>
-      <c r="C78" s="1" t="s">
-        <v>431</v>
-      </c>
-    </row>
-    <row r="79" spans="1:3">
-      <c r="A79" s="1" t="s">
-        <v>442</v>
-      </c>
-      <c r="B79" s="1" t="s">
-        <v>443</v>
-      </c>
-      <c r="C79" s="1" t="s">
-        <v>444</v>
-      </c>
-    </row>
-    <row r="80" spans="1:3">
+    </row>
+    <row r="80" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A80" s="1"/>
       <c r="B80" s="3"/>
       <c r="C80" s="1"/>
     </row>
-    <row r="81" spans="1:3">
+    <row r="81" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A81" s="1" t="s">
+        <v>442</v>
+      </c>
+      <c r="B81" s="1" t="s">
+        <v>443</v>
+      </c>
+      <c r="C81" s="1" t="s">
+        <v>444</v>
+      </c>
+    </row>
+    <row r="82" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A82" s="1" t="s">
         <v>445</v>
       </c>
-      <c r="B81" s="1" t="s">
+      <c r="B82" s="1" t="s">
         <v>446</v>
       </c>
-      <c r="C81" s="1" t="s">
+      <c r="C82" s="1" t="s">
         <v>447</v>
       </c>
     </row>
-    <row r="82" spans="1:3">
-      <c r="A82" s="1" t="s">
+    <row r="83" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A83" s="1" t="s">
         <v>448</v>
       </c>
-      <c r="B82" s="1" t="s">
+      <c r="B83" s="1" t="s">
         <v>449</v>
       </c>
-      <c r="C82" s="1" t="s">
+      <c r="C83" s="1" t="s">
         <v>450</v>
       </c>
     </row>
-    <row r="83" spans="1:3">
-      <c r="A83" s="1" t="s">
+    <row r="84" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A84" s="1" t="s">
         <v>451</v>
       </c>
-      <c r="B83" s="1" t="s">
+      <c r="B84" s="1" t="s">
         <v>452</v>
       </c>
-      <c r="C83" s="1" t="s">
+      <c r="C84" s="1" t="s">
         <v>453</v>
       </c>
     </row>
-    <row r="84" spans="1:3">
-      <c r="A84" s="1" t="s">
+    <row r="85" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A85" s="1" t="s">
         <v>454</v>
       </c>
-      <c r="B84" s="1" t="s">
+      <c r="B85" s="1" t="s">
         <v>455</v>
       </c>
-      <c r="C84" s="1" t="s">
+      <c r="C85" s="1" t="s">
         <v>456</v>
       </c>
     </row>
-    <row r="85" spans="1:3">
-      <c r="A85" s="1" t="s">
+    <row r="86" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A86" s="1" t="s">
         <v>457</v>
       </c>
-      <c r="B85" s="1" t="s">
+      <c r="B86" s="1" t="s">
         <v>458</v>
       </c>
-      <c r="C85" s="1" t="s">
+      <c r="C86" s="1" t="s">
         <v>459</v>
       </c>
     </row>
-    <row r="86" spans="1:3">
-      <c r="A86" s="1" t="s">
+    <row r="87" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A87" s="1" t="s">
         <v>460</v>
       </c>
-      <c r="B86" s="1" t="s">
+      <c r="B87" s="1" t="s">
         <v>461</v>
       </c>
-      <c r="C86" s="1" t="s">
+      <c r="C87" s="1" t="s">
         <v>462</v>
       </c>
     </row>
-    <row r="87" spans="1:3">
-      <c r="A87" s="1" t="s">
+    <row r="88" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A88" s="1" t="s">
+        <v>276</v>
+      </c>
+      <c r="B88" s="1" t="s">
         <v>463</v>
       </c>
-      <c r="B87" s="1" t="s">
+      <c r="C88" s="1" t="s">
         <v>464</v>
       </c>
-      <c r="C87" s="1" t="s">
+    </row>
+    <row r="89" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A89" s="1" t="s">
         <v>465</v>
       </c>
-    </row>
-    <row r="88" spans="1:3">
-      <c r="A88" s="1" t="s">
-        <v>279</v>
-      </c>
-      <c r="B88" s="1" t="s">
+      <c r="B89" s="1" t="s">
         <v>466</v>
       </c>
-      <c r="C88" s="1" t="s">
+      <c r="C89" s="1" t="s">
         <v>467</v>
       </c>
     </row>
-    <row r="89" spans="1:3">
-      <c r="A89" s="1" t="s">
+    <row r="90" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A90" s="1" t="s">
         <v>468</v>
       </c>
-      <c r="B89" s="1" t="s">
+      <c r="B90" s="1" t="s">
         <v>469</v>
       </c>
-      <c r="C89" s="1" t="s">
+      <c r="C90" s="1" t="s">
         <v>470</v>
-      </c>
-    </row>
-    <row r="90" spans="1:3">
-      <c r="A90" s="1" t="s">
-        <v>471</v>
-      </c>
-      <c r="B90" s="1" t="s">
-        <v>472</v>
-      </c>
-      <c r="C90" s="1" t="s">
-        <v>473</v>
       </c>
     </row>
   </sheetData>

</xml_diff>